<commit_message>
Add inference and visualization tests specification and implementation. Perform some adjustements and bug fixes.
</commit_message>
<xml_diff>
--- a/docs/test cases/authorization/AuthorizationTests.xlsx
+++ b/docs/test cases/authorization/AuthorizationTests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Projeto\PhyloDB\docs\test cases\authorization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Projeto\Project\PhyloDB\docs\test cases\authorization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22ECED1-0B38-4A49-B8AF-56BE079DCEDC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7382785-5A10-4DE6-8191-7CF48DBE69ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28935" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="31">
   <si>
     <t>Parameter</t>
   </si>
@@ -114,7 +114,16 @@
     <t>pre-handle</t>
   </si>
   <si>
-    <t xml:space="preserve">  + mandatory e non authorized</t>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Management, Algorithm</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
   </si>
 </sst>
 </file>
@@ -236,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -265,6 +274,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -279,9 +294,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,30 +575,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -597,8 +609,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -608,8 +620,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -619,8 +631,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -630,8 +642,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -641,8 +653,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -652,335 +664,643 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="6" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="7" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>4</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>5</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>6</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>7</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>8</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="9">
+        <v>10</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="9">
+        <v>11</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="9">
         <v>1</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D23" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="E23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="9">
         <v>2</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B24" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="D24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="9">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B25" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="E25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="B26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="9" t="s">
+      <c r="F26" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="H26" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="B27" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="9" t="s">
+      <c r="F27" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="H27" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="9">
+        <v>6</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="9" t="s">
+      <c r="F28" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="H28" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="9">
         <v>7</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="B29" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="9" t="s">
+      <c r="F29" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>8</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="H29" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="9">
+        <v>8</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="9" t="s">
+      <c r="F30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>9</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="H30" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="9">
+        <v>9</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="9" t="s">
+      <c r="F31" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
+      <c r="H31" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="9">
         <v>10</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="B32" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="9" t="s">
+      <c r="F32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
+      <c r="H32" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="9">
         <v>11</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="B33" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="9" t="s">
+      <c r="F33" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="38" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="39" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="40" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="41" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="42" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="45" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="H33" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="49" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="50" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="51" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1052,11 +1372,10 @@
     <row r="117" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="118" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="119" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="120" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>